<commit_message>
Initial commit: Complete Playwright testing framework
- RBL, IRC, and Sanity test suites
- Multi-environment support (QC2, QC3, QC6, UAT361)
- Page Object Model architecture
- Excel data-driven testing
- Allure reporting integration
- Comprehensive test utilities and configurations
</commit_message>
<xml_diff>
--- a/tests/data/RBL Test Data.xlsx
+++ b/tests/data/RBL Test Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="CategoryCreation" sheetId="1" state="visible" r:id="rId3"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="160">
   <si>
     <t xml:space="preserve">category</t>
   </si>
@@ -252,10 +252,10 @@
     <t xml:space="preserve">OTSPERCENTAGE</t>
   </si>
   <si>
-    <t xml:space="preserve">Branch name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Branchname</t>
+    <t xml:space="preserve">Existing Loan Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExistingLoanAmount</t>
   </si>
   <si>
     <t xml:space="preserve">PTP Date</t>
@@ -304,6 +304,57 @@
   </si>
   <si>
     <t xml:space="preserve">Need Discount,No discount,None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Contactable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CustomerContactable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes,No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If Customer not available on call mention Relationship with customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IfCustomernotavailableoncallmentionRelationshipwithcustomer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spouse,Parent,Sibling,Relative,Friend,Neighbor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IssueStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open,In Progress,Resolved,Closed,Pending Customer Confirmation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evidence confirmation available (as per telephonic confirmation by customer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evidenceconfirmationavailable(aspertelephonicconfirmationgivenbythecustomer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes,No,Pending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation Regular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ObservationRegular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Genuine,Discrepancy Found,To be Verified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Observation OD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ObservationOD</t>
   </si>
   <si>
     <t xml:space="preserve">PTPDate</t>
@@ -541,16 +592,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -794,27 +841,27 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>20</v>
@@ -849,18 +896,18 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -887,8 +934,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="12.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="10.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="10.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,24 +943,24 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -945,15 +992,15 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -985,21 +1032,21 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1020,48 +1067,55 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="13.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="12.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1069,10 +1123,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1104,19 +1158,19 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>12</v>
@@ -1167,45 +1221,45 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="23.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="16.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="43.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="23.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="43.99"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>124</v>
+      <c r="A2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1235,7 +1289,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -1244,80 +1298,80 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1488,27 +1542,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="4.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="8.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="24.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="4.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="4.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="8.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="12.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="7.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2199,6 +2253,32 @@
         <v>0</v>
       </c>
       <c r="H26" s="1" t="n">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>155</v>
       </c>
     </row>
@@ -2218,13 +2298,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="24.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.03"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2327,10 +2411,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
@@ -2914,6 +2998,32 @@
         <v>0</v>
       </c>
       <c r="H26" s="1" t="n">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <v>155</v>
       </c>
     </row>
@@ -2933,19 +3043,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="11.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,16 +3188,145 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="C6:D6"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3157,7 +3396,7 @@
         <v>73</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
@@ -3166,7 +3405,7 @@
         <v>75</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>77</v>
@@ -3270,21 +3509,21 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>20</v>

</xml_diff>